<commit_message>
update readme and a new picture
</commit_message>
<xml_diff>
--- a/project/exp.xlsx
+++ b/project/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/didwhddks/Desktop/2023-NTHU-Parallel-Programming/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C87A1F1-0B2F-C644-9573-21C2F1FC1B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ACD3C9-23A3-4141-BBC6-4CF9884C3576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17060" xr2:uid="{B4031528-6C7C-F24C-A0FA-E64244CB0D64}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>